<commit_message>
Updated data leaning example
</commit_message>
<xml_diff>
--- a/examples/04_Excel/data_cleaning/messy_data.xlsx
+++ b/examples/04_Excel/data_cleaning/messy_data.xlsx
@@ -1,12 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <bookViews>
+    <workbookView tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="messy" sheetId="1" r:id="rId4"/>
+    <sheet r:id="rId1" name="messy" sheetId="1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" iterateCount="100" iterateDelta="0.001"/>
 </workbook>
 </file>
 
@@ -73,52 +74,103 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10">
-    <font>
-      <sz val="10.0"/>
+  <fonts count="14">
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <b val="0"/>
+      <i val="0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <b/>
+      <i val="0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <b val="0"/>
+      <i val="0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
       <strike/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <i val="0"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <i val="0"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -128,23 +180,26 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF9900"/>
-        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="8">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -203,86 +258,71 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="1" applyAlignment="1"/>
   </cellStyleXfs>
   <cellXfs count="22">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="11" fillId="2" borderId="4" xfId="0"/>
+    <xf numFmtId="171" fontId="9" fillId="0" borderId="4" xfId="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="171" fontId="9" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="171" fontId="9" fillId="0" borderId="4" xfId="0"/>
+    <xf numFmtId="171" fontId="9" fillId="3" borderId="4" xfId="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="171" fontId="5" fillId="0" borderId="4" xfId="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="4" xfId="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="4" xfId="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -319,12 +359,12 @@
       <a:majorFont>
         <a:latin typeface="Arial"/>
         <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Arial"/>
         <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:cs typeface=""/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -336,149 +376,183 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{61488408-A3CD-A31F-C9DC-B2D44FCB67AD}" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:T200"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" defaultColWidth="14.421875" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -489,7 +563,7 @@
       <c r="F1" s="5"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
@@ -497,7 +571,7 @@
       <c r="E2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="6"/>
       <c r="B3" s="10" t="s">
         <v>1</v>
@@ -515,7 +589,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
         <v>4</v>
@@ -533,7 +607,7 @@
       <c r="I4" s="15"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="6"/>
       <c r="B5" s="6" t="s">
         <v>6</v>
@@ -551,7 +625,7 @@
       <c r="I5" s="15"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="6"/>
       <c r="B6" s="6" t="s">
         <v>9</v>
@@ -569,7 +643,7 @@
       <c r="I6" s="15"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="6" t="s">
         <v>10</v>
@@ -587,7 +661,7 @@
       <c r="I7" s="15"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="6"/>
       <c r="B8" s="6" t="s">
         <v>11</v>
@@ -605,7 +679,7 @@
       <c r="I8" s="15"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9">
+    <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="6"/>
       <c r="B9" s="6" t="s">
         <v>12</v>
@@ -623,7 +697,7 @@
       <c r="I9" s="15"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="6"/>
       <c r="B10" s="6" t="s">
         <v>13</v>
@@ -641,7 +715,7 @@
       <c r="I10" s="15"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="6"/>
       <c r="B11" s="10" t="s">
         <v>14</v>
@@ -659,7 +733,7 @@
       <c r="I11" s="15"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>15</v>
@@ -677,7 +751,7 @@
       <c r="I12" s="15"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="6"/>
       <c r="B13" s="6" t="s">
         <v>16</v>
@@ -695,7 +769,7 @@
       <c r="I13" s="15"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="6"/>
       <c r="B14" s="6" t="s">
         <v>17</v>
@@ -713,7 +787,7 @@
       <c r="I14" s="15"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15">
+    <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="6"/>
       <c r="B15" s="6" t="s">
         <v>18</v>
@@ -731,7 +805,7 @@
       <c r="I15" s="15"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -743,14 +817,14 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="21"/>
       <c r="E17" s="1"/>
       <c r="F17" s="21"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18">
+    <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -762,7 +836,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19">
+    <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -774,7 +848,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20">
+    <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -786,7 +860,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21">
+    <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -799,12 +873,19 @@
       <c r="J21" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells>
     <mergeCell ref="B1:D2"/>
     <mergeCell ref="F1:I2"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="F17:I17"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <printOptions/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;C&amp;R</oddHeader>
+    <oddFooter>&amp;L&amp;C&amp;R</oddFooter>
+  </headerFooter>
+  <extLst/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated data leaning example (#406)
</commit_message>
<xml_diff>
--- a/examples/04_Excel/data_cleaning/messy_data.xlsx
+++ b/examples/04_Excel/data_cleaning/messy_data.xlsx
@@ -1,12 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <bookViews>
+    <workbookView tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="messy" sheetId="1" r:id="rId4"/>
+    <sheet r:id="rId1" name="messy" sheetId="1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" iterateCount="100" iterateDelta="0.001"/>
 </workbook>
 </file>
 
@@ -73,52 +74,103 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10">
-    <font>
-      <sz val="10.0"/>
+  <fonts count="14">
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <b val="0"/>
+      <i val="0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <b/>
+      <i val="0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <b val="0"/>
+      <i val="0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
       <strike/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <i val="0"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <i val="0"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -128,23 +180,26 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF9900"/>
-        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="8">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -203,86 +258,71 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="1" applyAlignment="1"/>
   </cellStyleXfs>
   <cellXfs count="22">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="11" fillId="2" borderId="4" xfId="0"/>
+    <xf numFmtId="171" fontId="9" fillId="0" borderId="4" xfId="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="171" fontId="9" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="171" fontId="9" fillId="0" borderId="4" xfId="0"/>
+    <xf numFmtId="171" fontId="9" fillId="3" borderId="4" xfId="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="171" fontId="5" fillId="0" borderId="4" xfId="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="4" xfId="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="4" xfId="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -319,12 +359,12 @@
       <a:majorFont>
         <a:latin typeface="Arial"/>
         <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Arial"/>
         <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:cs typeface=""/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -336,149 +376,183 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{61488408-A3CD-A31F-C9DC-B2D44FCB67AD}" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:T200"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" defaultColWidth="14.421875" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -489,7 +563,7 @@
       <c r="F1" s="5"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
@@ -497,7 +571,7 @@
       <c r="E2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="6"/>
       <c r="B3" s="10" t="s">
         <v>1</v>
@@ -515,7 +589,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
         <v>4</v>
@@ -533,7 +607,7 @@
       <c r="I4" s="15"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="6"/>
       <c r="B5" s="6" t="s">
         <v>6</v>
@@ -551,7 +625,7 @@
       <c r="I5" s="15"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="6"/>
       <c r="B6" s="6" t="s">
         <v>9</v>
@@ -569,7 +643,7 @@
       <c r="I6" s="15"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="6" t="s">
         <v>10</v>
@@ -587,7 +661,7 @@
       <c r="I7" s="15"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="6"/>
       <c r="B8" s="6" t="s">
         <v>11</v>
@@ -605,7 +679,7 @@
       <c r="I8" s="15"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9">
+    <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="6"/>
       <c r="B9" s="6" t="s">
         <v>12</v>
@@ -623,7 +697,7 @@
       <c r="I9" s="15"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="6"/>
       <c r="B10" s="6" t="s">
         <v>13</v>
@@ -641,7 +715,7 @@
       <c r="I10" s="15"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="6"/>
       <c r="B11" s="10" t="s">
         <v>14</v>
@@ -659,7 +733,7 @@
       <c r="I11" s="15"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>15</v>
@@ -677,7 +751,7 @@
       <c r="I12" s="15"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="6"/>
       <c r="B13" s="6" t="s">
         <v>16</v>
@@ -695,7 +769,7 @@
       <c r="I13" s="15"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="6"/>
       <c r="B14" s="6" t="s">
         <v>17</v>
@@ -713,7 +787,7 @@
       <c r="I14" s="15"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15">
+    <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="6"/>
       <c r="B15" s="6" t="s">
         <v>18</v>
@@ -731,7 +805,7 @@
       <c r="I15" s="15"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -743,14 +817,14 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="21"/>
       <c r="E17" s="1"/>
       <c r="F17" s="21"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18">
+    <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -762,7 +836,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19">
+    <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -774,7 +848,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20">
+    <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -786,7 +860,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21">
+    <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -799,12 +873,19 @@
       <c r="J21" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells>
     <mergeCell ref="B1:D2"/>
     <mergeCell ref="F1:I2"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="F17:I17"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <printOptions/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;C&amp;R</oddHeader>
+    <oddFooter>&amp;L&amp;C&amp;R</oddFooter>
+  </headerFooter>
+  <extLst/>
 </worksheet>
 </file>
</xml_diff>